<commit_message>
I add  Team info and OMDB queries
</commit_message>
<xml_diff>
--- a/iteration_2_template.xlsx
+++ b/iteration_2_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_jasthi\Metro_Master_Do_Not_Delete\_ICS311_Database_Management_Systems\_Monday\Assignments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abdiali/Documents/GitHub/omdb/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F7F87E2-9B65-4ED0-A3AB-51FF9BB13924}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{385DE71C-F54D-6C48-99DD-09F1F68C48EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10300" yWindow="2780" windowWidth="23260" windowHeight="12580" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>Your Team Name</t>
   </si>
@@ -48,13 +48,67 @@
   </si>
   <si>
     <t>Scrum Master</t>
+  </si>
+  <si>
+    <t>Elephants</t>
+  </si>
+  <si>
+    <t>Abdi Ali</t>
+  </si>
+  <si>
+    <t>abdi.ali@my.metrostate.edu</t>
+  </si>
+  <si>
+    <t>612-6550830</t>
+  </si>
+  <si>
+    <t>Olukole Solabi</t>
+  </si>
+  <si>
+    <t>Ian Berube</t>
+  </si>
+  <si>
+    <t>Chris Cassens</t>
+  </si>
+  <si>
+    <t>Huy Dinh</t>
+  </si>
+  <si>
+    <t>Mohamed Abdirahman</t>
+  </si>
+  <si>
+    <t>Olaniyi Jayeola</t>
+  </si>
+  <si>
+    <t>A &amp; B</t>
+  </si>
+  <si>
+    <t>Get all movie name that were made in China.</t>
+  </si>
+  <si>
+    <t>A &amp; C</t>
+  </si>
+  <si>
+    <t>Get all movie name and year  that was directed by Sam Raimi</t>
+  </si>
+  <si>
+    <t>A &amp; E</t>
+  </si>
+  <si>
+    <t>Get movie name and movie poster for all movies that have more than one movie posters.</t>
+  </si>
+  <si>
+    <t>A , B &amp; D</t>
+  </si>
+  <si>
+    <t>Get  all audio link and song title from movies made in India in year between 1990 to 2000.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -189,6 +243,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF220011"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -371,7 +439,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -486,8 +554,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF1C3F4F"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF1C3F4F"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF1C3F4F"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF1C3F4F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -530,8 +613,9 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -540,8 +624,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -575,6 +663,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -898,32 +987,38 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:A11"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21" style="1" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" customWidth="1"/>
+    <col min="2" max="2" width="30.1640625" customWidth="1"/>
     <col min="3" max="3" width="21.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -934,44 +1029,53 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
-        <v>7</v>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B5" r:id="rId1" xr:uid="{1A3F50C3-D1B8-9941-B647-EDEC1313C8EB}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;LUnrestricted </oddFooter>
     <evenFooter xml:space="preserve">&amp;LUnrestricted </evenFooter>
@@ -985,16 +1089,16 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="27.33203125" customWidth="1"/>
-    <col min="3" max="3" width="68.5546875" customWidth="1"/>
+    <col min="3" max="3" width="68.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
@@ -1005,127 +1109,151 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B4" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B5" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>

</xml_diff>